<commit_message>
aggiornamento dell'analisi dei rischi Excel
</commit_message>
<xml_diff>
--- a/analisiDeiRiscihiEXCEL.xlsx
+++ b/analisiDeiRiscihiEXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Desktop\progettoGestione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45973E41-8AB9-4D06-BD32-1D7DA39BB4F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AB8076-F03F-4E92-A684-7CF5BF3CF610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,7 +331,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A9DF3BC1-9742-6741-902A-E2056DAAB984}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="12">
     <dxf>
       <font>
         <color auto="1"/>
@@ -422,96 +422,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -861,7 +771,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1002,7 +912,9 @@
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
       <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +943,9 @@
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
       <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +974,9 @@
       <c r="N6"/>
     </row>
     <row r="7" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
       <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1089,7 +1005,9 @@
       <c r="N7"/>
     </row>
     <row r="8" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
+      <c r="B8" s="11">
+        <v>6</v>
+      </c>
       <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1118,7 +1036,9 @@
       <c r="N8"/>
     </row>
     <row r="9" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
+      <c r="B9" s="11">
+        <v>7</v>
+      </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1418,13 +1338,13 @@
     <row r="36" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3:G9">
-    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="11" priority="27" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="10" priority="28" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",F3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>